<commit_message>
can not print first part of MOVE.L or MOVEA.L
</commit_message>
<xml_diff>
--- a/OpCodes.xlsx
+++ b/OpCodes.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_F25DC773A252ABEACE02ECE02B9864DE5ADE58A2" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{CACC4922-14D6-47FF-B185-D63144B6DE9E}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="11_F25DC773A252ABEACE02ECE02B9864DE5ADE58A2" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{25FB4153-F93F-4983-90F8-A75CCF810017}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179020"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>OpCode</t>
   </si>
@@ -152,9 +151,6 @@
   </si>
   <si>
     <t>Bcc (BGT, BLE, BEQ)</t>
-  </si>
-  <si>
-    <t>HEAD</t>
   </si>
 </sst>
 </file>
@@ -198,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -213,9 +209,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -973,349 +966,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB9992E-F9AD-4D68-8A34-D7D23BB5E30A}">
-  <dimension ref="D4:AB15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="4" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="N4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-    </row>
-    <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-    </row>
-    <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7">
-        <v>1</v>
-      </c>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-    </row>
-    <row r="8" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-    </row>
-    <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7">
-        <v>0</v>
-      </c>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7">
-        <v>1</v>
-      </c>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-    </row>
-    <row r="10" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-    </row>
-    <row r="11" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7">
-        <v>1</v>
-      </c>
-      <c r="J11" s="7">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7">
-        <v>1</v>
-      </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7">
-        <v>1</v>
-      </c>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7">
-        <v>0</v>
-      </c>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-    </row>
-    <row r="12" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-    </row>
-    <row r="13" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-    </row>
-    <row r="14" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-    </row>
-    <row r="15" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>